<commit_message>
Atualiza a base de dados e resultados
</commit_message>
<xml_diff>
--- a/data/Características Acadêmicas e Profissionais que Influenciam a Entrada em um Projeto no Curso de Ciência da Computação na UFCG (respostas).xlsx
+++ b/data/Características Acadêmicas e Profissionais que Influenciam a Entrada em um Projeto no Curso de Ciência da Computação na UFCG (respostas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="38">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Projetos pessoais (websites, aplicativos próprios e etc), Cursos externos (e.g. Udemy, Alura, Khanacademy, Skill Share, etc), Grupos de estudo, Competições independentes</t>
+  </si>
+  <si>
+    <t>Projetos pessoais (websites, aplicativos próprios e etc), Nenhuma</t>
+  </si>
+  <si>
+    <t>Participação em Eventos como Ouvinte, Em Curso ou Aprovado(a) em alguma disciplina de Didática</t>
   </si>
 </sst>
 </file>
@@ -128,17 +134,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,14 +172,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,10 +532,10 @@
       <c r="A7" s="5">
         <v>44293.73780209491</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -542,7 +544,7 @@
       <c r="E7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -550,10 +552,10 @@
       <c r="A8" s="5">
         <v>44293.818034537035</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -562,7 +564,7 @@
       <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -570,10 +572,10 @@
       <c r="A9" s="5">
         <v>44293.81862798611</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -582,7 +584,7 @@
       <c r="E9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -590,10 +592,10 @@
       <c r="A10" s="5">
         <v>44293.82432142361</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -602,7 +604,7 @@
       <c r="E10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -610,10 +612,10 @@
       <c r="A11" s="5">
         <v>44293.83126168982</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -622,7 +624,7 @@
       <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -630,10 +632,10 @@
       <c r="A12" s="5">
         <v>44294.878202569445</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -642,7 +644,7 @@
       <c r="E12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -656,10 +658,10 @@
       <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -676,10 +678,10 @@
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -696,10 +698,10 @@
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -716,10 +718,10 @@
       <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -736,10 +738,10 @@
       <c r="C17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -756,10 +758,10 @@
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -776,10 +778,10 @@
       <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -796,10 +798,10 @@
       <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -816,10 +818,10 @@
       <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -836,13 +838,73 @@
       <c r="C22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5">
+        <v>44301.4706641088</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5">
+        <v>44301.83158115741</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5">
+        <v>44303.43661967592</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>